<commit_message>
adiconado motorista e visual do campo obaservação
</commit_message>
<xml_diff>
--- a/data/motoristas.xlsx
+++ b/data/motoristas.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28829"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\tickets_entrega\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CE4470D-0F57-4B2F-8648-B571336BD71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD1CD2F-77BD-46DA-ADEC-4D4D8784FB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{5A27738C-59EF-4211-A28E-3F9EB786C10F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5A27738C-59EF-4211-A28E-3F9EB786C10F}"/>
   </bookViews>
   <sheets>
     <sheet name="motoristas" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">motoristas!$A$1:$A$3085</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="3074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3085" uniqueCount="3080">
   <si>
     <t>Motorista</t>
   </si>
@@ -9242,6 +9245,24 @@
   </si>
   <si>
     <t>ZEFERINO RODRIGUES DA SILVEIRA NETO</t>
+  </si>
+  <si>
+    <t>Motorista - SERRAVALE</t>
+  </si>
+  <si>
+    <t>Motorista - SERRANO</t>
+  </si>
+  <si>
+    <t>Motorista - JM</t>
+  </si>
+  <si>
+    <t>Motorista - AMARAL</t>
+  </si>
+  <si>
+    <t>Motorista - LAJEADENSE</t>
+  </si>
+  <si>
+    <t>Motorista - LANA TRANSPORTES</t>
   </si>
 </sst>
 </file>
@@ -10102,11 +10123,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E98EC2-7FAF-4B75-94DE-AFE0E88C8931}">
-  <dimension ref="A1:A3079"/>
+  <dimension ref="A1:A3085"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -21815,3695 +21841,3730 @@
     </row>
     <row r="2342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2342" t="s">
-        <v>2337</v>
+        <v>3077</v>
       </c>
     </row>
     <row r="2343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2343" t="s">
-        <v>2338</v>
+        <v>3076</v>
       </c>
     </row>
     <row r="2344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2344" t="s">
-        <v>2339</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="2345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2345" t="s">
-        <v>2340</v>
+        <v>3079</v>
       </c>
     </row>
     <row r="2346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2346" t="s">
-        <v>2341</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="2347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2347" t="s">
-        <v>2342</v>
+        <v>3074</v>
       </c>
     </row>
     <row r="2348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2348" t="s">
-        <v>2343</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="2349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2349" t="s">
-        <v>2344</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="2350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2350" t="s">
-        <v>2345</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="2351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2351" t="s">
-        <v>2346</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="2352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2352" t="s">
-        <v>2347</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="2353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2353" t="s">
-        <v>2348</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="2354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2354" t="s">
-        <v>2349</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="2355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2355" t="s">
-        <v>2350</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="2356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2356" t="s">
-        <v>2351</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="2357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2357" t="s">
-        <v>2352</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="2358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2358" t="s">
-        <v>2353</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="2359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2359" t="s">
-        <v>2354</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="2360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2360" t="s">
-        <v>2355</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="2361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2361" t="s">
-        <v>2356</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="2362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2362" t="s">
-        <v>2357</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="2363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2363" t="s">
-        <v>2358</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="2364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2364" t="s">
-        <v>2359</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="2365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2365" t="s">
-        <v>2360</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="2366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2366" t="s">
-        <v>2361</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="2367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2367" t="s">
-        <v>2362</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="2368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2368" t="s">
-        <v>2363</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="2369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2369" t="s">
-        <v>2364</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="2370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2370" t="s">
-        <v>2365</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="2371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2371" t="s">
-        <v>2366</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="2372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2372" t="s">
-        <v>2367</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="2373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2373" t="s">
-        <v>2368</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="2374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2374" t="s">
-        <v>2369</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="2375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2375" t="s">
-        <v>2370</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="2376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2376" t="s">
-        <v>2371</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="2377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2377" t="s">
-        <v>2372</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="2378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2378" t="s">
-        <v>2373</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="2379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2379" t="s">
-        <v>2374</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="2380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2380" t="s">
-        <v>2375</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="2381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2381" t="s">
-        <v>2376</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="2382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2382" t="s">
-        <v>2377</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="2383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2383" t="s">
-        <v>2378</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="2384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2384" t="s">
-        <v>2379</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="2385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2385" t="s">
-        <v>2380</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="2386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2386" t="s">
-        <v>2381</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="2387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2387" t="s">
-        <v>2382</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="2388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2388" t="s">
-        <v>2383</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="2389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2389" t="s">
-        <v>2384</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="2390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2390" t="s">
-        <v>2385</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="2391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2391" t="s">
-        <v>2386</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="2392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2392" t="s">
-        <v>2387</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="2393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2393" t="s">
-        <v>2388</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="2394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2394" t="s">
-        <v>2389</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="2395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2395" t="s">
-        <v>2390</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="2396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2396" t="s">
-        <v>2391</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="2397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2397" t="s">
-        <v>2392</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="2398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2398" t="s">
-        <v>2393</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="2399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2399" t="s">
-        <v>2394</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="2400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2400" t="s">
-        <v>2395</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="2401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2401" t="s">
-        <v>2396</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="2402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2402" t="s">
-        <v>2397</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="2403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2403" t="s">
-        <v>2398</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="2404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2404" t="s">
-        <v>2399</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="2405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2405" t="s">
-        <v>2400</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="2406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2406" t="s">
-        <v>2401</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="2407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2407" t="s">
-        <v>2402</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="2408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2408" t="s">
-        <v>2403</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="2409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2409" t="s">
-        <v>2404</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="2410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2410" t="s">
-        <v>2405</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="2411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2411" t="s">
-        <v>2406</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="2412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2412" t="s">
-        <v>2407</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="2413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2413" t="s">
-        <v>2408</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="2414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2414" t="s">
-        <v>2409</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="2415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2415" t="s">
-        <v>2410</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="2416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2416" t="s">
-        <v>2411</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="2417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2417" t="s">
-        <v>2412</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="2418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2418" t="s">
-        <v>2413</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="2419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2419" t="s">
-        <v>2414</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="2420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2420" t="s">
-        <v>2415</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="2421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2421" t="s">
-        <v>2416</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="2422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2422" t="s">
-        <v>2417</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="2423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2423" t="s">
-        <v>2418</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="2424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2424" t="s">
-        <v>2419</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="2425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2425" t="s">
-        <v>2420</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="2426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2426" t="s">
-        <v>2421</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="2427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2427" t="s">
-        <v>2422</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="2428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2428" t="s">
-        <v>2423</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="2429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2429" t="s">
-        <v>2424</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="2430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2430" t="s">
-        <v>2425</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="2431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2431" t="s">
-        <v>2426</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="2432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2432" t="s">
-        <v>2427</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="2433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2433" t="s">
-        <v>2428</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="2434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2434" t="s">
-        <v>2429</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="2435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2435" t="s">
-        <v>2430</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="2436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2436" t="s">
-        <v>2431</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="2437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2437" t="s">
-        <v>2432</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="2438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2438" t="s">
-        <v>2433</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="2439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2439" t="s">
-        <v>2434</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="2440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2440" t="s">
-        <v>2435</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="2441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2441" t="s">
-        <v>2436</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="2442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2442" t="s">
-        <v>2437</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="2443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2443" t="s">
-        <v>2438</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="2444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2444" t="s">
-        <v>2439</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="2445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2445" t="s">
-        <v>2440</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="2446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2446" t="s">
-        <v>2441</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="2447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2447" t="s">
-        <v>2442</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="2448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2448" t="s">
-        <v>2443</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="2449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2449" t="s">
-        <v>2444</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="2450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2450" t="s">
-        <v>2445</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="2451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2451" t="s">
-        <v>2446</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="2452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2452" t="s">
-        <v>2447</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="2453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2453" t="s">
-        <v>2448</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="2454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2454" t="s">
-        <v>2449</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2455" t="s">
-        <v>2450</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="2456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2456" t="s">
-        <v>2451</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="2457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2457" t="s">
-        <v>2452</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="2458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2458" t="s">
-        <v>2453</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="2459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2459" t="s">
-        <v>2454</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="2460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2460" t="s">
-        <v>2455</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="2461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2461" t="s">
-        <v>2456</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="2462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2462" t="s">
-        <v>2457</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="2463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2463" t="s">
-        <v>2458</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="2464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2464" t="s">
-        <v>2459</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="2465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2465" t="s">
-        <v>2460</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="2466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2466" t="s">
-        <v>2461</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="2467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2467" t="s">
-        <v>2462</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="2468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2468" t="s">
-        <v>2463</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="2469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2469" t="s">
-        <v>2464</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="2470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2470" t="s">
-        <v>2465</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="2471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2471" t="s">
-        <v>2466</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="2472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2472" t="s">
-        <v>2467</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="2473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2473" t="s">
-        <v>2468</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="2474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2474" t="s">
-        <v>2469</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="2475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2475" t="s">
-        <v>2470</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="2476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2476" t="s">
-        <v>2471</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="2477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2477" t="s">
-        <v>2472</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="2478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2478" t="s">
-        <v>2473</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="2479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2479" t="s">
-        <v>2474</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="2480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2480" t="s">
-        <v>2475</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="2481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2481" t="s">
-        <v>2476</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="2482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2482" t="s">
-        <v>2477</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="2483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2483" t="s">
-        <v>2478</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="2484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2484" t="s">
-        <v>2479</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="2485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2485" t="s">
-        <v>2480</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="2486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2486" t="s">
-        <v>2481</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="2487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2487" t="s">
-        <v>2482</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="2488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2488" t="s">
-        <v>2483</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="2489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2489" t="s">
-        <v>2484</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="2490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2490" t="s">
-        <v>2485</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="2491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2491" t="s">
-        <v>2486</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="2492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2492" t="s">
-        <v>2487</v>
+        <v>2481</v>
       </c>
     </row>
     <row r="2493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2493" t="s">
-        <v>2488</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="2494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2494" t="s">
-        <v>2489</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="2495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2495" t="s">
-        <v>2490</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="2496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2496" t="s">
-        <v>2491</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="2497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2497" t="s">
-        <v>2492</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="2498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2498" t="s">
-        <v>2493</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="2499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2499" t="s">
-        <v>2494</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="2500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2500" t="s">
-        <v>2495</v>
+        <v>2489</v>
       </c>
     </row>
     <row r="2501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2501" t="s">
-        <v>2496</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="2502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2502" t="s">
-        <v>2497</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="2503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2503" t="s">
-        <v>2498</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="2504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2504" t="s">
-        <v>2499</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="2505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2505" t="s">
-        <v>2500</v>
+        <v>2494</v>
       </c>
     </row>
     <row r="2506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2506" t="s">
-        <v>2501</v>
+        <v>2495</v>
       </c>
     </row>
     <row r="2507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2507" t="s">
-        <v>2502</v>
+        <v>2496</v>
       </c>
     </row>
     <row r="2508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2508" t="s">
-        <v>2503</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="2509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2509" t="s">
-        <v>2504</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="2510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2510" t="s">
-        <v>2505</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="2511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2511" t="s">
-        <v>2506</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="2512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2512" t="s">
-        <v>2507</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="2513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2513" t="s">
-        <v>2508</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="2514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2514" t="s">
-        <v>2509</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="2515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2515" t="s">
-        <v>2510</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="2516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2516" t="s">
-        <v>2511</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="2517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2517" t="s">
-        <v>2512</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="2518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2518" t="s">
-        <v>2513</v>
+        <v>2507</v>
       </c>
     </row>
     <row r="2519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2519" t="s">
-        <v>2514</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="2520" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2520" t="s">
-        <v>2515</v>
+        <v>2509</v>
       </c>
     </row>
     <row r="2521" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2521" t="s">
-        <v>2516</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="2522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2522" t="s">
-        <v>2517</v>
+        <v>2511</v>
       </c>
     </row>
     <row r="2523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2523" t="s">
-        <v>2518</v>
+        <v>2512</v>
       </c>
     </row>
     <row r="2524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2524" t="s">
-        <v>2519</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="2525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2525" t="s">
-        <v>2520</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="2526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2526" t="s">
-        <v>2521</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="2527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2527" t="s">
-        <v>2522</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="2528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2528" t="s">
-        <v>2523</v>
+        <v>2517</v>
       </c>
     </row>
     <row r="2529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2529" t="s">
-        <v>2524</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="2530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2530" t="s">
-        <v>2525</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="2531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2531" t="s">
-        <v>2526</v>
+        <v>2520</v>
       </c>
     </row>
     <row r="2532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2532" t="s">
-        <v>2527</v>
+        <v>2521</v>
       </c>
     </row>
     <row r="2533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2533" t="s">
-        <v>2528</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="2534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2534" t="s">
-        <v>2529</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="2535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2535" t="s">
-        <v>2530</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="2536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2536" t="s">
-        <v>2531</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="2537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2537" t="s">
-        <v>2532</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="2538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2538" t="s">
-        <v>2533</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="2539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2539" t="s">
-        <v>2534</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="2540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2540" t="s">
-        <v>2535</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="2541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2541" t="s">
-        <v>2536</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="2542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2542" t="s">
-        <v>2537</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="2543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2543" t="s">
-        <v>2538</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="2544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2544" t="s">
-        <v>2539</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="2545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2545" t="s">
-        <v>2540</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="2546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2546" t="s">
-        <v>2541</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="2547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2547" t="s">
-        <v>2542</v>
+        <v>2536</v>
       </c>
     </row>
     <row r="2548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2548" t="s">
-        <v>2543</v>
+        <v>2537</v>
       </c>
     </row>
     <row r="2549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2549" t="s">
-        <v>2544</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="2550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2550" t="s">
-        <v>2545</v>
+        <v>2539</v>
       </c>
     </row>
     <row r="2551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2551" t="s">
-        <v>2546</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="2552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2552" t="s">
-        <v>2547</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="2553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2553" t="s">
-        <v>2548</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="2554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2554" t="s">
-        <v>2549</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="2555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2555" t="s">
-        <v>2550</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="2556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2556" t="s">
-        <v>2551</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="2557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2557" t="s">
-        <v>2552</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="2558" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2558" t="s">
-        <v>2553</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="2559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2559" t="s">
-        <v>2554</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="2560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2560" t="s">
-        <v>2555</v>
+        <v>2549</v>
       </c>
     </row>
     <row r="2561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2561" t="s">
-        <v>2556</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="2562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2562" t="s">
-        <v>2557</v>
+        <v>2551</v>
       </c>
     </row>
     <row r="2563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2563" t="s">
-        <v>2558</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="2564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2564" t="s">
-        <v>2559</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="2565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2565" t="s">
-        <v>2560</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="2566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2566" t="s">
-        <v>2561</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="2567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2567" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="2568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2568" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="2569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2569" t="s">
-        <v>2564</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="2570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2570" t="s">
-        <v>2565</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="2571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2571" t="s">
-        <v>2566</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="2572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2572" t="s">
-        <v>2567</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="2573" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2573" t="s">
-        <v>2568</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="2574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2574" t="s">
-        <v>2569</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="2575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2575" t="s">
-        <v>2570</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="2576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2576" t="s">
-        <v>2571</v>
+        <v>2565</v>
       </c>
     </row>
     <row r="2577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2577" t="s">
-        <v>2572</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="2578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2578" t="s">
-        <v>2573</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="2579" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2579" t="s">
-        <v>2574</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="2580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2580" t="s">
-        <v>2575</v>
+        <v>2569</v>
       </c>
     </row>
     <row r="2581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2581" t="s">
-        <v>2576</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="2582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2582" t="s">
-        <v>2577</v>
+        <v>2571</v>
       </c>
     </row>
     <row r="2583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2583" t="s">
-        <v>2578</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="2584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2584" t="s">
-        <v>2579</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="2585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2585" t="s">
-        <v>2580</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="2586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2586" t="s">
-        <v>2581</v>
+        <v>2575</v>
       </c>
     </row>
     <row r="2587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2587" t="s">
-        <v>2582</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="2588" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2588" t="s">
-        <v>2583</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="2589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2589" t="s">
-        <v>2584</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="2590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2590" t="s">
-        <v>2585</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="2591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2591" t="s">
-        <v>2586</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="2592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2592" t="s">
-        <v>2587</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="2593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2593" t="s">
-        <v>2588</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="2594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2594" t="s">
-        <v>2589</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="2595" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2595" t="s">
-        <v>2590</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="2596" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2596" t="s">
-        <v>2591</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="2597" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2597" t="s">
-        <v>2592</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="2598" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2598" t="s">
-        <v>2593</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="2599" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2599" t="s">
-        <v>2594</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="2600" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2600" t="s">
-        <v>2595</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="2601" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2601" t="s">
-        <v>2596</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="2602" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2602" t="s">
-        <v>2597</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="2603" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2603" t="s">
-        <v>2598</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="2604" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2604" t="s">
-        <v>2599</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="2605" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2605" t="s">
-        <v>2600</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="2606" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2606" t="s">
-        <v>2601</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="2607" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2607" t="s">
-        <v>2602</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="2608" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2608" t="s">
-        <v>2603</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="2609" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2609" t="s">
-        <v>2604</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="2610" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2610" t="s">
-        <v>2605</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="2611" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2611" t="s">
-        <v>2606</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="2612" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2612" t="s">
-        <v>2607</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="2613" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2613" t="s">
-        <v>2608</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="2614" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2614" t="s">
-        <v>2609</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="2615" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2615" t="s">
-        <v>2610</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="2616" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2616" t="s">
-        <v>2611</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="2617" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2617" t="s">
-        <v>2612</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="2618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2618" t="s">
-        <v>2613</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="2619" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2619" t="s">
-        <v>2614</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="2620" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2620" t="s">
-        <v>2615</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="2621" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2621" t="s">
-        <v>2616</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="2622" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2622" t="s">
-        <v>2617</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="2623" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2623" t="s">
-        <v>2618</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="2624" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2624" t="s">
-        <v>2619</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="2625" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2625" t="s">
-        <v>2620</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="2626" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2626" t="s">
-        <v>2621</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="2627" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2627" t="s">
-        <v>2622</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="2628" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2628" t="s">
-        <v>2623</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="2629" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2629" t="s">
-        <v>2624</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="2630" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2630" t="s">
-        <v>2625</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="2631" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2631" t="s">
-        <v>2626</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="2632" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2632" t="s">
-        <v>2627</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="2633" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2633" t="s">
-        <v>2628</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="2634" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2634" t="s">
-        <v>2629</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="2635" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2635" t="s">
-        <v>2630</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="2636" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2636" t="s">
-        <v>2631</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="2637" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2637" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="2638" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2638" t="s">
-        <v>2633</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="2639" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2639" t="s">
-        <v>2634</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="2640" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2640" t="s">
-        <v>2635</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="2641" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2641" t="s">
-        <v>2636</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="2642" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2642" t="s">
-        <v>2637</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="2643" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2643" t="s">
-        <v>2638</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="2644" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2644" t="s">
-        <v>2639</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="2645" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2645" t="s">
-        <v>2640</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="2646" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2646" t="s">
-        <v>2641</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="2647" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2647" t="s">
-        <v>2642</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="2648" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2648" t="s">
-        <v>2643</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="2649" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2649" t="s">
-        <v>2644</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="2650" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2650" t="s">
-        <v>2645</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="2651" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2651" t="s">
-        <v>2646</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="2652" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2652" t="s">
-        <v>2647</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="2653" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2653" t="s">
-        <v>2648</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="2654" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2654" t="s">
-        <v>2649</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="2655" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2655" t="s">
-        <v>2650</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="2656" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2656" t="s">
-        <v>2651</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="2657" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2657" t="s">
-        <v>2652</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="2658" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2658" t="s">
-        <v>2653</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="2659" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2659" t="s">
-        <v>2654</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="2660" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2660" t="s">
-        <v>2655</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="2661" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2661" t="s">
-        <v>2656</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="2662" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2662" t="s">
-        <v>2657</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="2663" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2663" t="s">
-        <v>2658</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="2664" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2664" t="s">
-        <v>2659</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="2665" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2665" t="s">
-        <v>2660</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="2666" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2666" t="s">
-        <v>2661</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="2667" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2667" t="s">
-        <v>2662</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="2668" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2668" t="s">
-        <v>2663</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="2669" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2669" t="s">
-        <v>2664</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="2670" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2670" t="s">
-        <v>2665</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="2671" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2671" t="s">
-        <v>2666</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="2672" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2672" t="s">
-        <v>2667</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="2673" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2673" t="s">
-        <v>2668</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="2674" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2674" t="s">
-        <v>2669</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="2675" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2675" t="s">
-        <v>2670</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="2676" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2676" t="s">
-        <v>2671</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="2677" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2677" t="s">
-        <v>2672</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="2678" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2678" t="s">
-        <v>2673</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="2679" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2679" t="s">
-        <v>2674</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="2680" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2680" t="s">
-        <v>2675</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="2681" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2681" t="s">
-        <v>2676</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="2682" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2682" t="s">
-        <v>2677</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="2683" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2683" t="s">
-        <v>2678</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="2684" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2684" t="s">
-        <v>2679</v>
+        <v>2673</v>
       </c>
     </row>
     <row r="2685" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2685" t="s">
-        <v>2680</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="2686" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2686" t="s">
-        <v>2681</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="2687" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2687" t="s">
-        <v>2682</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="2688" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2688" t="s">
-        <v>2683</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="2689" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2689" t="s">
-        <v>2684</v>
+        <v>2678</v>
       </c>
     </row>
     <row r="2690" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2690" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="2691" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2691" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="2692" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2692" t="s">
-        <v>2687</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="2693" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2693" t="s">
-        <v>2688</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="2694" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2694" t="s">
-        <v>2689</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="2695" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2695" t="s">
-        <v>2690</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="2696" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2696" t="s">
-        <v>2691</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="2697" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2697" t="s">
-        <v>2692</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="2698" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2698" t="s">
-        <v>2693</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="2699" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2699" t="s">
-        <v>2694</v>
+        <v>2688</v>
       </c>
     </row>
     <row r="2700" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2700" t="s">
-        <v>2695</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="2701" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2701" t="s">
-        <v>2696</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="2702" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2702" t="s">
-        <v>2697</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="2703" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2703" t="s">
-        <v>2698</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="2704" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2704" t="s">
-        <v>2699</v>
+        <v>2693</v>
       </c>
     </row>
     <row r="2705" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2705" t="s">
-        <v>2700</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="2706" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2706" t="s">
-        <v>2701</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="2707" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2707" t="s">
-        <v>2702</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="2708" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2708" t="s">
-        <v>2703</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="2709" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2709" t="s">
-        <v>2704</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="2710" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2710" t="s">
-        <v>2705</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="2711" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2711" t="s">
-        <v>2706</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="2712" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2712" t="s">
-        <v>2707</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="2713" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2713" t="s">
-        <v>2708</v>
+        <v>2702</v>
       </c>
     </row>
     <row r="2714" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2714" t="s">
-        <v>2709</v>
+        <v>2703</v>
       </c>
     </row>
     <row r="2715" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2715" t="s">
-        <v>2710</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="2716" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2716" t="s">
-        <v>2711</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="2717" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2717" t="s">
-        <v>2712</v>
+        <v>2706</v>
       </c>
     </row>
     <row r="2718" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2718" t="s">
-        <v>2713</v>
+        <v>2707</v>
       </c>
     </row>
     <row r="2719" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2719" t="s">
-        <v>2714</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="2720" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2720" t="s">
-        <v>2715</v>
+        <v>2709</v>
       </c>
     </row>
     <row r="2721" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2721" t="s">
-        <v>2716</v>
+        <v>2710</v>
       </c>
     </row>
     <row r="2722" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2722" t="s">
-        <v>2717</v>
+        <v>2711</v>
       </c>
     </row>
     <row r="2723" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2723" t="s">
-        <v>2718</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="2724" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2724" t="s">
-        <v>2719</v>
+        <v>2713</v>
       </c>
     </row>
     <row r="2725" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2725" t="s">
-        <v>2720</v>
+        <v>2714</v>
       </c>
     </row>
     <row r="2726" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2726" t="s">
-        <v>2721</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="2727" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2727" t="s">
-        <v>2722</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="2728" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2728" t="s">
-        <v>2723</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="2729" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2729" t="s">
-        <v>2724</v>
+        <v>2718</v>
       </c>
     </row>
     <row r="2730" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2730" t="s">
-        <v>2725</v>
+        <v>2719</v>
       </c>
     </row>
     <row r="2731" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2731" t="s">
-        <v>2726</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="2732" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2732" t="s">
-        <v>2727</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="2733" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2733" t="s">
-        <v>2728</v>
+        <v>2722</v>
       </c>
     </row>
     <row r="2734" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2734" t="s">
-        <v>2729</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="2735" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2735" t="s">
-        <v>2730</v>
+        <v>2724</v>
       </c>
     </row>
     <row r="2736" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2736" t="s">
-        <v>2731</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="2737" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2737" t="s">
-        <v>2732</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="2738" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2738" t="s">
-        <v>2733</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="2739" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2739" t="s">
-        <v>2734</v>
+        <v>2728</v>
       </c>
     </row>
     <row r="2740" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2740" t="s">
-        <v>2735</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="2741" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2741" t="s">
-        <v>2736</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="2742" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2742" t="s">
-        <v>2737</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="2743" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2743" t="s">
-        <v>2738</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="2744" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2744" t="s">
-        <v>2739</v>
+        <v>2733</v>
       </c>
     </row>
     <row r="2745" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2745" t="s">
-        <v>2740</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="2746" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2746" t="s">
-        <v>2741</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="2747" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2747" t="s">
-        <v>2742</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="2748" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2748" t="s">
-        <v>2743</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="2749" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2749" t="s">
-        <v>2744</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="2750" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2750" t="s">
-        <v>2745</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="2751" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2751" t="s">
-        <v>2746</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="2752" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2752" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
     </row>
     <row r="2753" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2753" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="2754" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2754" t="s">
-        <v>2749</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="2755" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2755" t="s">
-        <v>2750</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="2756" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2756" t="s">
-        <v>2751</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="2757" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2757" t="s">
-        <v>2752</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="2758" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2758" t="s">
-        <v>2753</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="2759" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2759" t="s">
-        <v>2754</v>
+        <v>2748</v>
       </c>
     </row>
     <row r="2760" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2760" t="s">
-        <v>2755</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="2761" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2761" t="s">
-        <v>2756</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="2762" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2762" t="s">
-        <v>2757</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="2763" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2763" t="s">
-        <v>2758</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="2764" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2764" t="s">
-        <v>2759</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="2765" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2765" t="s">
-        <v>2760</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="2766" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2766" t="s">
-        <v>2761</v>
+        <v>2755</v>
       </c>
     </row>
     <row r="2767" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2767" t="s">
-        <v>2762</v>
+        <v>2756</v>
       </c>
     </row>
     <row r="2768" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2768" t="s">
-        <v>2763</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="2769" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2769" t="s">
-        <v>2764</v>
+        <v>2758</v>
       </c>
     </row>
     <row r="2770" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2770" t="s">
-        <v>2765</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="2771" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2771" t="s">
-        <v>2766</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="2772" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2772" t="s">
-        <v>2767</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="2773" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2773" t="s">
-        <v>2768</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="2774" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2774" t="s">
-        <v>2769</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="2775" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2775" t="s">
-        <v>2770</v>
+        <v>2764</v>
       </c>
     </row>
     <row r="2776" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2776" t="s">
-        <v>2771</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="2777" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2777" t="s">
-        <v>2772</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="2778" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2778" t="s">
-        <v>2773</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="2779" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2779" t="s">
-        <v>2774</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="2780" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2780" t="s">
-        <v>2775</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="2781" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2781" t="s">
-        <v>2776</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="2782" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2782" t="s">
-        <v>2777</v>
+        <v>2771</v>
       </c>
     </row>
     <row r="2783" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2783" t="s">
-        <v>2778</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="2784" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2784" t="s">
-        <v>2779</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="2785" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2785" t="s">
-        <v>2780</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="2786" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2786" t="s">
-        <v>2781</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="2787" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2787" t="s">
-        <v>2782</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="2788" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2788" t="s">
-        <v>2783</v>
+        <v>2777</v>
       </c>
     </row>
     <row r="2789" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2789" t="s">
-        <v>2784</v>
+        <v>2778</v>
       </c>
     </row>
     <row r="2790" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2790" t="s">
-        <v>2785</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="2791" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2791" t="s">
-        <v>2786</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="2792" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2792" t="s">
-        <v>2787</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="2793" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2793" t="s">
-        <v>2788</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="2794" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2794" t="s">
-        <v>2789</v>
+        <v>2783</v>
       </c>
     </row>
     <row r="2795" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2795" t="s">
-        <v>2790</v>
+        <v>2784</v>
       </c>
     </row>
     <row r="2796" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2796" t="s">
-        <v>2791</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="2797" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2797" t="s">
-        <v>2792</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="2798" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2798" t="s">
-        <v>2793</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="2799" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2799" t="s">
-        <v>2794</v>
+        <v>2788</v>
       </c>
     </row>
     <row r="2800" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2800" t="s">
-        <v>2795</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="2801" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2801" t="s">
-        <v>2796</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="2802" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2802" t="s">
-        <v>2797</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="2803" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2803" t="s">
-        <v>2798</v>
+        <v>2792</v>
       </c>
     </row>
     <row r="2804" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2804" t="s">
-        <v>2799</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="2805" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2805" t="s">
-        <v>2800</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="2806" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2806" t="s">
-        <v>2801</v>
+        <v>2795</v>
       </c>
     </row>
     <row r="2807" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2807" t="s">
-        <v>2802</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="2808" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2808" t="s">
-        <v>2803</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="2809" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2809" t="s">
-        <v>2804</v>
+        <v>2798</v>
       </c>
     </row>
     <row r="2810" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2810" t="s">
-        <v>2805</v>
+        <v>2799</v>
       </c>
     </row>
     <row r="2811" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2811" t="s">
-        <v>2806</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="2812" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2812" t="s">
-        <v>2807</v>
+        <v>2801</v>
       </c>
     </row>
     <row r="2813" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2813" t="s">
-        <v>2808</v>
+        <v>2802</v>
       </c>
     </row>
     <row r="2814" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2814" t="s">
-        <v>2809</v>
+        <v>2803</v>
       </c>
     </row>
     <row r="2815" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2815" t="s">
-        <v>2810</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="2816" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2816" t="s">
-        <v>2811</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="2817" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2817" t="s">
-        <v>2812</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="2818" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2818" t="s">
-        <v>2813</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="2819" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2819" t="s">
-        <v>2814</v>
+        <v>2808</v>
       </c>
     </row>
     <row r="2820" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2820" t="s">
-        <v>2815</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="2821" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2821" t="s">
-        <v>2816</v>
+        <v>2810</v>
       </c>
     </row>
     <row r="2822" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2822" t="s">
-        <v>2817</v>
+        <v>2811</v>
       </c>
     </row>
     <row r="2823" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2823" t="s">
-        <v>2818</v>
+        <v>2812</v>
       </c>
     </row>
     <row r="2824" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2824" t="s">
-        <v>2819</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="2825" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2825" t="s">
-        <v>2820</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="2826" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2826" t="s">
-        <v>2821</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="2827" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2827" t="s">
-        <v>2822</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="2828" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2828" t="s">
-        <v>2823</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="2829" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2829" t="s">
-        <v>2824</v>
+        <v>2818</v>
       </c>
     </row>
     <row r="2830" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2830" t="s">
-        <v>2825</v>
+        <v>2819</v>
       </c>
     </row>
     <row r="2831" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2831" t="s">
-        <v>2826</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="2832" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2832" t="s">
-        <v>2827</v>
+        <v>2821</v>
       </c>
     </row>
     <row r="2833" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2833" t="s">
-        <v>2828</v>
+        <v>2822</v>
       </c>
     </row>
     <row r="2834" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2834" t="s">
-        <v>2829</v>
+        <v>2823</v>
       </c>
     </row>
     <row r="2835" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2835" t="s">
-        <v>2830</v>
+        <v>2824</v>
       </c>
     </row>
     <row r="2836" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2836" t="s">
-        <v>2831</v>
+        <v>2825</v>
       </c>
     </row>
     <row r="2837" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2837" t="s">
-        <v>2832</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="2838" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2838" t="s">
-        <v>2833</v>
+        <v>2827</v>
       </c>
     </row>
     <row r="2839" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2839" t="s">
-        <v>2834</v>
+        <v>2828</v>
       </c>
     </row>
     <row r="2840" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2840" t="s">
-        <v>2835</v>
+        <v>2829</v>
       </c>
     </row>
     <row r="2841" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2841" t="s">
-        <v>2836</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="2842" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2842" t="s">
-        <v>2837</v>
+        <v>2831</v>
       </c>
     </row>
     <row r="2843" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2843" t="s">
-        <v>2838</v>
+        <v>2832</v>
       </c>
     </row>
     <row r="2844" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2844" t="s">
-        <v>2839</v>
+        <v>2833</v>
       </c>
     </row>
     <row r="2845" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2845" t="s">
-        <v>2840</v>
+        <v>2834</v>
       </c>
     </row>
     <row r="2846" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2846" t="s">
-        <v>2841</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="2847" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2847" t="s">
-        <v>2842</v>
+        <v>2836</v>
       </c>
     </row>
     <row r="2848" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2848" t="s">
-        <v>2843</v>
+        <v>2837</v>
       </c>
     </row>
     <row r="2849" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2849" t="s">
-        <v>2844</v>
+        <v>2838</v>
       </c>
     </row>
     <row r="2850" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2850" t="s">
-        <v>2845</v>
+        <v>2839</v>
       </c>
     </row>
     <row r="2851" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2851" t="s">
-        <v>2846</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="2852" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2852" t="s">
-        <v>2847</v>
+        <v>2841</v>
       </c>
     </row>
     <row r="2853" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2853" t="s">
-        <v>2848</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="2854" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2854" t="s">
-        <v>2849</v>
+        <v>2843</v>
       </c>
     </row>
     <row r="2855" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2855" t="s">
-        <v>2850</v>
+        <v>2844</v>
       </c>
     </row>
     <row r="2856" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2856" t="s">
-        <v>2851</v>
+        <v>2845</v>
       </c>
     </row>
     <row r="2857" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2857" t="s">
-        <v>2852</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="2858" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2858" t="s">
-        <v>2853</v>
+        <v>2847</v>
       </c>
     </row>
     <row r="2859" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2859" t="s">
-        <v>2854</v>
+        <v>2848</v>
       </c>
     </row>
     <row r="2860" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2860" t="s">
-        <v>2855</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="2861" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2861" t="s">
-        <v>2856</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="2862" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2862" t="s">
-        <v>2857</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="2863" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2863" t="s">
-        <v>2858</v>
+        <v>2852</v>
       </c>
     </row>
     <row r="2864" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2864" t="s">
-        <v>2859</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="2865" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2865" t="s">
-        <v>2860</v>
+        <v>2854</v>
       </c>
     </row>
     <row r="2866" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2866" t="s">
-        <v>2861</v>
+        <v>2855</v>
       </c>
     </row>
     <row r="2867" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2867" t="s">
-        <v>2862</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="2868" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2868" t="s">
-        <v>2863</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="2869" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2869" t="s">
-        <v>2864</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="2870" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2870" t="s">
-        <v>2865</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="2871" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2871" t="s">
-        <v>2866</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="2872" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2872" t="s">
-        <v>2867</v>
+        <v>2861</v>
       </c>
     </row>
     <row r="2873" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2873" t="s">
-        <v>2868</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="2874" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2874" t="s">
-        <v>2869</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="2875" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2875" t="s">
-        <v>2870</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="2876" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2876" t="s">
-        <v>2871</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="2877" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2877" t="s">
-        <v>2872</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="2878" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2878" t="s">
-        <v>2873</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="2879" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2879" t="s">
-        <v>2874</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="2880" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2880" t="s">
-        <v>2875</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="2881" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2881" t="s">
-        <v>2876</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="2882" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2882" t="s">
-        <v>2877</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="2883" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2883" t="s">
-        <v>2878</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="2884" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2884" t="s">
-        <v>2879</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="2885" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2885" t="s">
-        <v>2880</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="2886" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2886" t="s">
-        <v>2881</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="2887" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2887" t="s">
-        <v>2882</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="2888" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2888" t="s">
-        <v>2883</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="2889" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2889" t="s">
-        <v>2884</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="2890" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2890" t="s">
-        <v>2885</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="2891" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2891" t="s">
-        <v>2886</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="2892" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2892" t="s">
-        <v>2887</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="2893" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2893" t="s">
-        <v>2888</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="2894" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2894" t="s">
-        <v>2889</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="2895" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2895" t="s">
-        <v>2890</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="2896" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2896" t="s">
-        <v>2891</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="2897" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2897" t="s">
-        <v>2892</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="2898" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2898" t="s">
-        <v>2893</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="2899" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2899" t="s">
-        <v>2894</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="2900" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2900" t="s">
-        <v>2895</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="2901" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2901" t="s">
-        <v>2896</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="2902" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2902" t="s">
-        <v>2897</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="2903" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2903" t="s">
-        <v>2898</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="2904" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2904" t="s">
-        <v>2899</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="2905" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2905" t="s">
-        <v>2900</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="2906" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2906" t="s">
-        <v>2901</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="2907" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2907" t="s">
-        <v>2902</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="2908" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2908" t="s">
-        <v>2903</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="2909" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2909" t="s">
-        <v>2904</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="2910" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2910" t="s">
-        <v>2905</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="2911" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2911" t="s">
-        <v>2906</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="2912" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2912" t="s">
-        <v>2907</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="2913" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2913" t="s">
-        <v>2908</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="2914" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2914" t="s">
-        <v>2909</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="2915" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2915" t="s">
-        <v>2910</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="2916" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2916" t="s">
-        <v>2911</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="2917" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2917" t="s">
-        <v>2912</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="2918" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2918" t="s">
-        <v>2913</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="2919" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2919" t="s">
-        <v>2914</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="2920" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2920" t="s">
-        <v>2915</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="2921" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2921" t="s">
-        <v>2916</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="2922" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2922" t="s">
-        <v>2917</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="2923" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2923" t="s">
-        <v>2918</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="2924" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2924" t="s">
-        <v>2919</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="2925" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2925" t="s">
-        <v>2920</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="2926" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2926" t="s">
-        <v>2921</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="2927" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2927" t="s">
-        <v>2922</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="2928" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2928" t="s">
-        <v>2923</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="2929" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2929" t="s">
-        <v>2924</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="2930" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2930" t="s">
-        <v>2925</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="2931" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2931" t="s">
-        <v>2926</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="2932" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2932" t="s">
-        <v>2927</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="2933" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2933" t="s">
-        <v>2928</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="2934" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2934" t="s">
-        <v>2929</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="2935" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2935" t="s">
-        <v>2930</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="2936" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2936" t="s">
-        <v>2931</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="2937" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2937" t="s">
-        <v>2932</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="2938" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2938" t="s">
-        <v>2933</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="2939" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2939" t="s">
-        <v>2934</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="2940" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2940" t="s">
-        <v>2935</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="2941" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2941" t="s">
-        <v>2936</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="2942" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2942" t="s">
-        <v>2937</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="2943" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2943" t="s">
-        <v>2938</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="2944" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2944" t="s">
-        <v>2939</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="2945" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2945" t="s">
-        <v>2940</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="2946" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2946" t="s">
-        <v>2941</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="2947" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2947" t="s">
-        <v>2942</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="2948" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2948" t="s">
-        <v>2943</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="2949" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2949" t="s">
-        <v>2944</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="2950" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2950" t="s">
-        <v>2945</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="2951" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2951" t="s">
-        <v>2946</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="2952" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2952" t="s">
-        <v>2947</v>
+        <v>2941</v>
       </c>
     </row>
     <row r="2953" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2953" t="s">
-        <v>2948</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="2954" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2954" t="s">
-        <v>2949</v>
+        <v>2943</v>
       </c>
     </row>
     <row r="2955" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2955" t="s">
-        <v>2950</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="2956" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2956" t="s">
-        <v>2951</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="2957" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2957" t="s">
-        <v>2952</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="2958" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2958" t="s">
-        <v>2953</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="2959" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2959" t="s">
-        <v>2954</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="2960" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2960" t="s">
-        <v>2955</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="2961" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2961" t="s">
-        <v>2956</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="2962" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2962" t="s">
-        <v>2957</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="2963" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2963" t="s">
-        <v>2958</v>
+        <v>2952</v>
       </c>
     </row>
     <row r="2964" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2964" t="s">
-        <v>2959</v>
+        <v>2953</v>
       </c>
     </row>
     <row r="2965" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2965" t="s">
-        <v>2960</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="2966" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2966" t="s">
-        <v>2961</v>
+        <v>2955</v>
       </c>
     </row>
     <row r="2967" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2967" t="s">
-        <v>2962</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="2968" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2968" t="s">
-        <v>2963</v>
+        <v>2957</v>
       </c>
     </row>
     <row r="2969" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2969" t="s">
-        <v>2964</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="2970" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2970" t="s">
-        <v>2965</v>
+        <v>2959</v>
       </c>
     </row>
     <row r="2971" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2971" t="s">
-        <v>2966</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="2972" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2972" t="s">
-        <v>2967</v>
+        <v>2961</v>
       </c>
     </row>
     <row r="2973" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2973" t="s">
-        <v>2968</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="2974" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2974" t="s">
-        <v>2969</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="2975" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2975" t="s">
-        <v>2970</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="2976" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2976" t="s">
-        <v>2971</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="2977" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2977" t="s">
-        <v>2972</v>
+        <v>2966</v>
       </c>
     </row>
     <row r="2978" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2978" t="s">
-        <v>2973</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="2979" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2979" t="s">
-        <v>2974</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="2980" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2980" t="s">
-        <v>2975</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="2981" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2981" t="s">
-        <v>2976</v>
+        <v>2970</v>
       </c>
     </row>
     <row r="2982" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2982" t="s">
-        <v>2977</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="2983" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2983" t="s">
-        <v>2978</v>
+        <v>2972</v>
       </c>
     </row>
     <row r="2984" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2984" t="s">
-        <v>2979</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="2985" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2985" t="s">
-        <v>2980</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="2986" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2986" t="s">
-        <v>2981</v>
+        <v>2975</v>
       </c>
     </row>
     <row r="2987" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2987" t="s">
-        <v>2982</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="2988" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2988" t="s">
-        <v>2983</v>
+        <v>2977</v>
       </c>
     </row>
     <row r="2989" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2989" t="s">
-        <v>2984</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="2990" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2990" t="s">
-        <v>2985</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="2991" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2991" t="s">
-        <v>2986</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="2992" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2992" t="s">
-        <v>2987</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="2993" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2993" t="s">
-        <v>2988</v>
+        <v>2982</v>
       </c>
     </row>
     <row r="2994" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2994" t="s">
-        <v>2989</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="2995" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2995" t="s">
-        <v>2990</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="2996" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2996" t="s">
-        <v>2991</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="2997" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2997" t="s">
-        <v>2992</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="2998" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2998" t="s">
-        <v>2993</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="2999" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2999" t="s">
-        <v>2994</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="3000" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3000" t="s">
-        <v>2995</v>
+        <v>2989</v>
       </c>
     </row>
     <row r="3001" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3001" t="s">
-        <v>2996</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="3002" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3002" t="s">
-        <v>2997</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="3003" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3003" t="s">
-        <v>2998</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="3004" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3004" t="s">
-        <v>2999</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="3005" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3005" t="s">
-        <v>3000</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="3006" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3006" t="s">
-        <v>3000</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="3007" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3007" t="s">
-        <v>3001</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="3008" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3008" t="s">
-        <v>3002</v>
+        <v>2997</v>
       </c>
     </row>
     <row r="3009" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3009" t="s">
-        <v>3003</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="3010" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3010" t="s">
-        <v>3004</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="3011" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3011" t="s">
-        <v>3005</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3012" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3012" t="s">
-        <v>3006</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3013" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3013" t="s">
-        <v>3007</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="3014" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3014" t="s">
-        <v>3008</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="3015" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3015" t="s">
-        <v>3009</v>
+        <v>3003</v>
       </c>
     </row>
     <row r="3016" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3016" t="s">
-        <v>3010</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="3017" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3017" t="s">
-        <v>3011</v>
+        <v>3005</v>
       </c>
     </row>
     <row r="3018" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3018" t="s">
-        <v>3012</v>
+        <v>3006</v>
       </c>
     </row>
     <row r="3019" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3019" t="s">
-        <v>3013</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="3020" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3020" t="s">
-        <v>3014</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="3021" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3021" t="s">
-        <v>3015</v>
+        <v>3009</v>
       </c>
     </row>
     <row r="3022" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3022" t="s">
-        <v>3016</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="3023" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3023" t="s">
-        <v>3017</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="3024" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3024" t="s">
-        <v>3018</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="3025" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3025" t="s">
-        <v>3019</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="3026" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3026" t="s">
-        <v>3020</v>
+        <v>3014</v>
       </c>
     </row>
     <row r="3027" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3027" t="s">
-        <v>3021</v>
+        <v>3015</v>
       </c>
     </row>
     <row r="3028" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3028" t="s">
-        <v>3022</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="3029" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3029" t="s">
-        <v>3023</v>
+        <v>3017</v>
       </c>
     </row>
     <row r="3030" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3030" t="s">
-        <v>3024</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="3031" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3031" t="s">
-        <v>3025</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="3032" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3032" t="s">
-        <v>3026</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="3033" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3033" t="s">
-        <v>3027</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="3034" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3034" t="s">
-        <v>3028</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="3035" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3035" t="s">
-        <v>3029</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="3036" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3036" t="s">
-        <v>3030</v>
+        <v>3024</v>
       </c>
     </row>
     <row r="3037" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3037" t="s">
-        <v>3031</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="3038" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3038" t="s">
-        <v>3032</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="3039" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3039" t="s">
-        <v>3033</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="3040" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3040" t="s">
-        <v>3034</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="3041" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3041" t="s">
-        <v>3035</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="3042" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3042" t="s">
-        <v>3036</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="3043" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3043" t="s">
-        <v>3037</v>
+        <v>3031</v>
       </c>
     </row>
     <row r="3044" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3044" t="s">
-        <v>3038</v>
+        <v>3032</v>
       </c>
     </row>
     <row r="3045" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3045" t="s">
-        <v>3039</v>
+        <v>3033</v>
       </c>
     </row>
     <row r="3046" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3046" t="s">
-        <v>3040</v>
+        <v>3034</v>
       </c>
     </row>
     <row r="3047" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3047" t="s">
-        <v>3041</v>
+        <v>3035</v>
       </c>
     </row>
     <row r="3048" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3048" t="s">
-        <v>3042</v>
+        <v>3036</v>
       </c>
     </row>
     <row r="3049" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3049" t="s">
-        <v>3043</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="3050" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3050" t="s">
-        <v>3044</v>
+        <v>3038</v>
       </c>
     </row>
     <row r="3051" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3051" t="s">
-        <v>3045</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="3052" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3052" t="s">
-        <v>3046</v>
+        <v>3040</v>
       </c>
     </row>
     <row r="3053" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3053" t="s">
-        <v>3047</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="3054" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3054" t="s">
-        <v>3048</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="3055" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3055" t="s">
-        <v>3049</v>
+        <v>3043</v>
       </c>
     </row>
     <row r="3056" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3056" t="s">
-        <v>3050</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="3057" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3057" t="s">
-        <v>3051</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="3058" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3058" t="s">
-        <v>3052</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="3059" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3059" t="s">
-        <v>3053</v>
+        <v>3047</v>
       </c>
     </row>
     <row r="3060" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3060" t="s">
-        <v>3054</v>
+        <v>3048</v>
       </c>
     </row>
     <row r="3061" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3061" t="s">
-        <v>3055</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="3062" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3062" t="s">
-        <v>3056</v>
+        <v>3050</v>
       </c>
     </row>
     <row r="3063" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3063" t="s">
-        <v>3057</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="3064" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3064" t="s">
-        <v>3058</v>
+        <v>3052</v>
       </c>
     </row>
     <row r="3065" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3065" t="s">
-        <v>3059</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="3066" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3066" t="s">
-        <v>3060</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="3067" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3067" t="s">
-        <v>3061</v>
+        <v>3055</v>
       </c>
     </row>
     <row r="3068" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3068" t="s">
-        <v>3062</v>
+        <v>3056</v>
       </c>
     </row>
     <row r="3069" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3069" t="s">
-        <v>3063</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="3070" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3070" t="s">
-        <v>3064</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="3071" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3071" t="s">
-        <v>3065</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="3072" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3072" t="s">
-        <v>3066</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="3073" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3073" t="s">
-        <v>3067</v>
+        <v>3061</v>
       </c>
     </row>
     <row r="3074" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3074" t="s">
-        <v>3068</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="3075" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3075" t="s">
-        <v>3069</v>
+        <v>3063</v>
       </c>
     </row>
     <row r="3076" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3076" t="s">
-        <v>3070</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="3077" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3077" t="s">
-        <v>3071</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="3078" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3078" t="s">
-        <v>3072</v>
+        <v>3066</v>
       </c>
     </row>
     <row r="3079" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3079" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="3080" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3080" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="3081" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3081" t="s">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="3082" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3082" t="s">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="3083" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3083" t="s">
+        <v>3071</v>
+      </c>
+    </row>
+    <row r="3084" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3084" t="s">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="3085" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3085" t="s">
         <v>3073</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A3085" xr:uid="{A0E98EC2-7FAF-4B75-94DE-AFE0E88C8931}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A3085">
+      <sortCondition ref="A1:A3085"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>